<commit_message>
fixed typo in thermodynamics. plotting extended output
</commit_message>
<xml_diff>
--- a/faster/Metadaten_all_86_cleanandneat.xlsx
+++ b/faster/Metadaten_all_86_cleanandneat.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lara\Desktop\simple model\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive - Universität Hamburg\simple model\faster\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -16,14 +16,14 @@
   </sheets>
   <definedNames>
     <definedName name="_13CGC_C.wke">#REF!</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Zusammenf. Permafrost Data'!$B$16:$H$21</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Zusammenf. Permafrost Data'!$B$16:$H$22</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="19">
   <si>
     <t>depth</t>
   </si>
@@ -165,7 +165,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyFont="1"/>
@@ -213,6 +213,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="11">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -527,10 +528,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q102"/>
+  <dimension ref="A1:Q103"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q30" sqref="Q30"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -538,12 +541,12 @@
     <col min="1" max="1" width="9" style="1"/>
     <col min="2" max="2" width="26.3984375" style="1" customWidth="1"/>
     <col min="3" max="3" width="27.296875" style="27" customWidth="1"/>
-    <col min="4" max="4" width="12.09765625" style="1" hidden="1" customWidth="1"/>
-    <col min="5" max="9" width="9" style="1" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="12.3984375" style="1" hidden="1" customWidth="1"/>
-    <col min="11" max="13" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="15.5" style="1" hidden="1" customWidth="1"/>
-    <col min="15" max="15" width="0" style="1" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="12.09765625" style="1" customWidth="1"/>
+    <col min="5" max="9" width="9" style="1" customWidth="1"/>
+    <col min="10" max="10" width="12.3984375" style="1" customWidth="1"/>
+    <col min="11" max="13" width="9" style="1" customWidth="1"/>
+    <col min="14" max="14" width="15.5" style="1" customWidth="1"/>
+    <col min="15" max="15" width="9" style="1" customWidth="1"/>
     <col min="16" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
@@ -778,10 +781,10 @@
         <v>8729.3203883495153</v>
       </c>
       <c r="P5" s="1">
-        <v>0</v>
+        <v>10.8</v>
       </c>
       <c r="Q5" s="1">
-        <v>0</v>
+        <v>8.92</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
@@ -832,10 +835,10 @@
         <v>16630</v>
       </c>
       <c r="P6" s="1">
-        <v>0</v>
+        <v>13.88</v>
       </c>
       <c r="Q6" s="1">
-        <v>0</v>
+        <v>5.4</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
@@ -886,10 +889,10 @@
         <v>16544.85436893204</v>
       </c>
       <c r="P7" s="1">
-        <v>0</v>
+        <v>12.5</v>
       </c>
       <c r="Q7" s="1">
-        <v>0</v>
+        <v>7.5</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
@@ -940,10 +943,10 @@
         <v>22056.369785794814</v>
       </c>
       <c r="P8" s="1">
-        <v>0</v>
+        <v>13.4</v>
       </c>
       <c r="Q8" s="1">
-        <v>0</v>
+        <v>5.9</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
@@ -990,10 +993,10 @@
         <v>23420.518602029311</v>
       </c>
       <c r="P9" s="1">
-        <v>0</v>
+        <v>8.35</v>
       </c>
       <c r="Q9" s="1">
-        <v>0</v>
+        <v>2.8</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
@@ -1044,10 +1047,10 @@
         <v>26813.979706877115</v>
       </c>
       <c r="P10" s="1">
-        <v>0</v>
+        <v>15.49</v>
       </c>
       <c r="Q10" s="1">
-        <v>0</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
@@ -1098,10 +1101,10 @@
         <v>29091.319052987601</v>
       </c>
       <c r="P11" s="1">
-        <v>0</v>
+        <v>14.15</v>
       </c>
       <c r="Q11" s="1">
-        <v>0</v>
+        <v>5.85</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
@@ -1152,10 +1155,10 @@
         <v>34333.7091319053</v>
       </c>
       <c r="P12" s="1">
-        <v>0</v>
+        <v>9.6300000000000008</v>
       </c>
       <c r="Q12" s="1">
-        <v>0</v>
+        <v>8.6300000000000008</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
@@ -1200,10 +1203,10 @@
         <v>36239.007891770008</v>
       </c>
       <c r="P13" s="1">
-        <v>0</v>
+        <v>13.5</v>
       </c>
       <c r="Q13" s="1">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
@@ -1248,10 +1251,10 @@
         <v>40000</v>
       </c>
       <c r="P14" s="1">
-        <v>0</v>
+        <v>11.38</v>
       </c>
       <c r="Q14" s="1">
-        <v>0</v>
+        <v>8.67</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
@@ -1296,10 +1299,10 @@
         <v>41639.233370913193</v>
       </c>
       <c r="P15" s="1">
-        <v>0</v>
+        <v>15.37</v>
       </c>
       <c r="Q15" s="1">
-        <v>0</v>
+        <v>3.55</v>
       </c>
     </row>
     <row r="16" spans="1:17" ht="15" x14ac:dyDescent="0.25">
@@ -1322,7 +1325,7 @@
         <v>4.7649999999999997</v>
       </c>
       <c r="G16" s="7">
-        <f t="shared" ref="G16:G21" si="1">F16/H16</f>
+        <f t="shared" ref="G16:G22" si="1">F16/H16</f>
         <v>12.441253263707571</v>
       </c>
       <c r="H16" s="6">
@@ -1350,10 +1353,10 @@
         <v>38000</v>
       </c>
       <c r="P16" s="1">
-        <v>0</v>
+        <v>9.7799999999999994</v>
       </c>
       <c r="Q16" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:17" ht="15" x14ac:dyDescent="0.25">
@@ -1405,10 +1408,10 @@
         <v>38900.315000000002</v>
       </c>
       <c r="P17" s="1">
-        <v>0</v>
+        <v>11.5</v>
       </c>
       <c r="Q17" s="1">
-        <v>0</v>
+        <v>8.8000000000000007</v>
       </c>
     </row>
     <row r="18" spans="1:17" ht="15" x14ac:dyDescent="0.25">
@@ -1513,10 +1516,10 @@
         <v>21770</v>
       </c>
       <c r="P19" s="1">
-        <v>0</v>
+        <v>12.3</v>
       </c>
       <c r="Q19" s="1">
-        <v>0</v>
+        <v>9.9</v>
       </c>
     </row>
     <row r="20" spans="1:17" ht="15" x14ac:dyDescent="0.25">
@@ -1575,103 +1578,100 @@
     </row>
     <row r="21" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B21" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21" s="28">
+        <v>1371</v>
+      </c>
+      <c r="D21" s="1">
+        <v>19.5</v>
+      </c>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6">
+        <v>0.76700000000000002</v>
+      </c>
+      <c r="G21" s="7">
+        <v>19</v>
+      </c>
+      <c r="H21" s="6">
+        <v>0.04</v>
+      </c>
+      <c r="I21" s="8">
+        <v>5.95</v>
+      </c>
+      <c r="J21" s="13">
+        <v>-27.23</v>
+      </c>
+      <c r="K21" s="13">
+        <v>0.09</v>
+      </c>
+      <c r="L21" s="10"/>
+      <c r="M21" s="10"/>
+      <c r="N21" s="31">
+        <v>19</v>
+      </c>
+      <c r="P21" s="1">
+        <v>17</v>
+      </c>
+      <c r="Q21" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" ht="15" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B21" s="17" t="s">
+      <c r="B22" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="C21" s="28">
+      <c r="C22" s="28">
         <v>1370</v>
       </c>
-      <c r="D21" s="1">
+      <c r="D22" s="1">
         <v>343.63799999999998</v>
       </c>
-      <c r="E21" s="6">
+      <c r="E22" s="6">
         <v>5.7000000000000002E-2</v>
       </c>
-      <c r="F21" s="6">
+      <c r="F22" s="6">
         <v>3.5720000000000001</v>
       </c>
-      <c r="G21" s="7">
+      <c r="G22" s="7">
         <f t="shared" si="1"/>
         <v>13.479245283018868</v>
       </c>
-      <c r="H21" s="6">
+      <c r="H22" s="6">
         <v>0.26500000000000001</v>
       </c>
-      <c r="I21" s="8">
+      <c r="I22" s="8">
         <v>7.17</v>
       </c>
-      <c r="J21" s="13">
+      <c r="J22" s="13">
         <v>-26.875400000000006</v>
       </c>
-      <c r="K21" s="13">
+      <c r="K22" s="13">
         <v>4.1999999999999815E-2</v>
       </c>
-      <c r="L21" s="10">
+      <c r="L22" s="10">
         <v>-26.170500000000001</v>
       </c>
-      <c r="M21" s="10">
+      <c r="M22" s="10">
         <v>2.7499999999999858E-2</v>
       </c>
-      <c r="N21">
+      <c r="N22">
         <v>30.95</v>
       </c>
-      <c r="O21" s="1">
+      <c r="O22" s="1">
         <v>14488.446601941747</v>
       </c>
-      <c r="P21" s="1">
+      <c r="P22" s="1">
         <v>13.81</v>
       </c>
-      <c r="Q21" s="1">
+      <c r="Q22" s="1">
         <v>6.2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B22" s="26" t="s">
-        <v>15</v>
-      </c>
-      <c r="C22" s="29">
-        <v>1372</v>
-      </c>
-      <c r="D22" s="20">
-        <v>69</v>
-      </c>
-      <c r="E22" s="5"/>
-      <c r="F22" s="6">
-        <v>0.59599999999999997</v>
-      </c>
-      <c r="G22" s="7">
-        <f t="shared" ref="G22:G30" si="2">F22/H22</f>
-        <v>16.108108108108109</v>
-      </c>
-      <c r="H22" s="5">
-        <v>3.6999999999999998E-2</v>
-      </c>
-      <c r="I22" s="5">
-        <v>6.15</v>
-      </c>
-      <c r="J22" s="10">
-        <v>-27.302321671555141</v>
-      </c>
-      <c r="K22" s="10">
-        <v>0.1481855998736121</v>
-      </c>
-      <c r="M22" s="11"/>
-      <c r="N22" s="14">
-        <v>20.96</v>
-      </c>
-      <c r="O22" s="1">
-        <v>45.220700000000022</v>
-      </c>
-      <c r="P22" s="1">
-        <v>17.77</v>
-      </c>
-      <c r="Q22" s="1">
-        <v>4.5999999999999996</v>
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
@@ -1682,43 +1682,43 @@
         <v>15</v>
       </c>
       <c r="C23" s="29">
-        <v>1373</v>
+        <v>1372</v>
       </c>
       <c r="D23" s="20">
-        <v>87.5</v>
+        <v>69</v>
       </c>
       <c r="E23" s="5"/>
       <c r="F23" s="6">
-        <v>1.3839999999999999</v>
+        <v>0.59599999999999997</v>
       </c>
       <c r="G23" s="7">
-        <f t="shared" si="2"/>
-        <v>21.968253968253965</v>
+        <f t="shared" ref="G23:G31" si="2">F23/H23</f>
+        <v>16.108108108108109</v>
       </c>
       <c r="H23" s="5">
-        <v>6.3E-2</v>
+        <v>3.6999999999999998E-2</v>
       </c>
       <c r="I23" s="5">
-        <v>6.08</v>
+        <v>6.15</v>
       </c>
       <c r="J23" s="10">
-        <v>-26.974370898974932</v>
+        <v>-27.302321671555141</v>
       </c>
       <c r="K23" s="10">
-        <v>0.39112449197405913</v>
+        <v>0.1481855998736121</v>
       </c>
       <c r="M23" s="11"/>
       <c r="N23" s="14">
-        <v>31.97</v>
+        <v>20.96</v>
       </c>
       <c r="O23" s="1">
-        <v>175</v>
+        <v>45.220700000000022</v>
       </c>
       <c r="P23" s="1">
-        <v>14.226000000000001</v>
+        <v>17.77</v>
       </c>
       <c r="Q23" s="1">
-        <v>6.6</v>
+        <v>4.5999999999999996</v>
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
@@ -1729,43 +1729,43 @@
         <v>15</v>
       </c>
       <c r="C24" s="29">
-        <v>1374</v>
+        <v>1373</v>
       </c>
       <c r="D24" s="20">
-        <v>146.5</v>
+        <v>87.5</v>
       </c>
       <c r="E24" s="5"/>
       <c r="F24" s="6">
-        <v>4.593</v>
+        <v>1.3839999999999999</v>
       </c>
       <c r="G24" s="7">
         <f t="shared" si="2"/>
-        <v>25.659217877094974</v>
+        <v>21.968253968253965</v>
       </c>
       <c r="H24" s="5">
-        <v>0.17899999999999999</v>
+        <v>6.3E-2</v>
       </c>
       <c r="I24" s="5">
-        <v>5.98</v>
+        <v>6.08</v>
       </c>
       <c r="J24" s="10">
-        <v>-25.94114964772762</v>
+        <v>-26.974370898974932</v>
       </c>
       <c r="K24" s="10">
-        <v>0.27357341515108302</v>
+        <v>0.39112449197405913</v>
       </c>
       <c r="M24" s="11"/>
       <c r="N24" s="14">
-        <v>64.260000000000005</v>
+        <v>31.97</v>
       </c>
       <c r="O24" s="1">
-        <v>578.44395000000009</v>
+        <v>175</v>
       </c>
       <c r="P24" s="1">
-        <v>7.44</v>
+        <v>14.226000000000001</v>
       </c>
       <c r="Q24" s="1">
-        <v>13</v>
+        <v>6.6</v>
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
@@ -1776,43 +1776,43 @@
         <v>15</v>
       </c>
       <c r="C25" s="29">
-        <v>1375</v>
+        <v>1374</v>
       </c>
       <c r="D25" s="20">
-        <v>201.5</v>
+        <v>146.5</v>
       </c>
       <c r="E25" s="5"/>
       <c r="F25" s="6">
-        <v>4.3630000000000004</v>
+        <v>4.593</v>
       </c>
       <c r="G25" s="7">
         <f t="shared" si="2"/>
-        <v>22.260204081632654</v>
+        <v>25.659217877094974</v>
       </c>
       <c r="H25" s="5">
-        <v>0.19600000000000001</v>
+        <v>0.17899999999999999</v>
       </c>
       <c r="I25" s="5">
-        <v>5.77</v>
+        <v>5.98</v>
       </c>
       <c r="J25" s="10">
-        <v>-27.399044480058059</v>
+        <v>-25.94114964772762</v>
       </c>
       <c r="K25" s="10">
-        <v>0.31061981511955555</v>
+        <v>0.27357341515108302</v>
       </c>
       <c r="M25" s="11"/>
       <c r="N25" s="14">
-        <v>53.44</v>
+        <v>64.260000000000005</v>
       </c>
       <c r="O25" s="1">
-        <v>956.86045000000013</v>
+        <v>578.44395000000009</v>
       </c>
       <c r="P25" s="1">
-        <v>9.9600000000000009</v>
+        <v>7.44</v>
       </c>
       <c r="Q25" s="1">
-        <v>11.5</v>
+        <v>13</v>
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
@@ -1823,50 +1823,43 @@
         <v>15</v>
       </c>
       <c r="C26" s="29">
-        <v>1376</v>
+        <v>1375</v>
       </c>
       <c r="D26" s="20">
-        <v>220</v>
-      </c>
-      <c r="E26" s="5">
-        <v>3.9E-2</v>
-      </c>
+        <v>201.5</v>
+      </c>
+      <c r="E26" s="5"/>
       <c r="F26" s="6">
-        <v>6.78</v>
+        <v>4.3630000000000004</v>
       </c>
       <c r="G26" s="7">
         <f t="shared" si="2"/>
-        <v>22.675585284280938</v>
+        <v>22.260204081632654</v>
       </c>
       <c r="H26" s="5">
-        <v>0.29899999999999999</v>
+        <v>0.19600000000000001</v>
       </c>
       <c r="I26" s="5">
-        <v>5.99</v>
-      </c>
-      <c r="J26" s="13">
-        <v>-28.075900000000004</v>
-      </c>
-      <c r="K26" s="13">
-        <v>8.1500000000000128E-2</v>
-      </c>
-      <c r="L26" s="10">
-        <v>-27.584</v>
-      </c>
-      <c r="M26" s="10">
-        <v>0.1509999999999998</v>
-      </c>
+        <v>5.77</v>
+      </c>
+      <c r="J26" s="10">
+        <v>-27.399044480058059</v>
+      </c>
+      <c r="K26" s="10">
+        <v>0.31061981511955555</v>
+      </c>
+      <c r="M26" s="11"/>
       <c r="N26" s="14">
-        <v>53.9</v>
+        <v>53.44</v>
       </c>
       <c r="O26" s="1">
-        <v>1080</v>
+        <v>956.86045000000013</v>
       </c>
       <c r="P26" s="1">
-        <v>0</v>
+        <v>9.9600000000000009</v>
       </c>
       <c r="Q26" s="1">
-        <v>0</v>
+        <v>11.5</v>
       </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
@@ -1876,51 +1869,51 @@
       <c r="B27" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="C27" s="30">
-        <v>1377</v>
-      </c>
-      <c r="D27" s="2">
-        <v>290.5</v>
+      <c r="C27" s="29">
+        <v>1376</v>
+      </c>
+      <c r="D27" s="20">
+        <v>220</v>
       </c>
       <c r="E27" s="5">
-        <v>7.0000000000000007E-2</v>
+        <v>3.9E-2</v>
       </c>
       <c r="F27" s="6">
-        <v>4.8289999999999997</v>
+        <v>6.78</v>
       </c>
       <c r="G27" s="7">
         <f t="shared" si="2"/>
-        <v>23.788177339901473</v>
+        <v>22.675585284280938</v>
       </c>
       <c r="H27" s="5">
-        <v>0.20300000000000001</v>
+        <v>0.29899999999999999</v>
       </c>
       <c r="I27" s="5">
-        <v>6.42</v>
+        <v>5.99</v>
       </c>
       <c r="J27" s="13">
-        <v>-26.649400000000007</v>
+        <v>-28.075900000000004</v>
       </c>
       <c r="K27" s="13">
-        <v>1.9000000000000128E-2</v>
+        <v>8.1500000000000128E-2</v>
       </c>
       <c r="L27" s="10">
-        <v>-25.863500000000002</v>
+        <v>-27.584</v>
       </c>
       <c r="M27" s="10">
-        <v>0.11650000000000027</v>
+        <v>0.1509999999999998</v>
       </c>
       <c r="N27" s="14">
-        <v>52.63</v>
+        <v>53.9</v>
       </c>
       <c r="O27" s="1">
-        <v>1569.20715</v>
+        <v>1080</v>
       </c>
       <c r="P27" s="1">
-        <v>9.67</v>
+        <v>10.72</v>
       </c>
       <c r="Q27" s="1">
-        <v>10.5</v>
+        <v>12.5</v>
       </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
@@ -1931,50 +1924,50 @@
         <v>15</v>
       </c>
       <c r="C28" s="30">
-        <v>1378</v>
+        <v>1377</v>
       </c>
       <c r="D28" s="2">
-        <v>327</v>
+        <v>290.5</v>
       </c>
       <c r="E28" s="5">
-        <v>9.4E-2</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="F28" s="6">
-        <v>4.04</v>
+        <v>4.8289999999999997</v>
       </c>
       <c r="G28" s="7">
         <f t="shared" si="2"/>
-        <v>19.238095238095237</v>
+        <v>23.788177339901473</v>
       </c>
       <c r="H28" s="5">
-        <v>0.21</v>
+        <v>0.20300000000000001</v>
       </c>
       <c r="I28" s="5">
-        <v>6.37</v>
+        <v>6.42</v>
       </c>
       <c r="J28" s="13">
-        <v>-26.620400000000004</v>
+        <v>-26.649400000000007</v>
       </c>
       <c r="K28" s="13">
-        <v>1.2000000000000455E-2</v>
+        <v>1.9000000000000128E-2</v>
       </c>
       <c r="L28" s="10">
-        <v>-25.95</v>
+        <v>-25.863500000000002</v>
       </c>
       <c r="M28" s="10">
-        <v>0.12700000000000067</v>
+        <v>0.11650000000000027</v>
       </c>
       <c r="N28" s="14">
-        <v>59.89</v>
+        <v>52.63</v>
       </c>
       <c r="O28" s="1">
-        <v>1820.3380999999999</v>
+        <v>1569.20715</v>
       </c>
       <c r="P28" s="1">
-        <v>8.66</v>
+        <v>9.67</v>
       </c>
       <c r="Q28" s="1">
-        <v>13</v>
+        <v>10.5</v>
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
@@ -1985,50 +1978,50 @@
         <v>15</v>
       </c>
       <c r="C29" s="30">
-        <v>1379</v>
+        <v>1378</v>
       </c>
       <c r="D29" s="2">
-        <v>379.5</v>
+        <v>327</v>
       </c>
       <c r="E29" s="5">
-        <v>5.0999999999999997E-2</v>
+        <v>9.4E-2</v>
       </c>
       <c r="F29" s="6">
-        <v>3.16</v>
+        <v>4.04</v>
       </c>
       <c r="G29" s="7">
         <f t="shared" si="2"/>
-        <v>14.905660377358492</v>
+        <v>19.238095238095237</v>
       </c>
       <c r="H29" s="5">
-        <v>0.21199999999999999</v>
+        <v>0.21</v>
       </c>
       <c r="I29" s="5">
-        <v>6.57</v>
+        <v>6.37</v>
       </c>
       <c r="J29" s="13">
-        <v>-26.973900000000008</v>
+        <v>-26.620400000000004</v>
       </c>
       <c r="K29" s="13">
-        <v>1.4499999999999957E-2</v>
+        <v>1.2000000000000455E-2</v>
       </c>
       <c r="L29" s="10">
-        <v>-26.406500000000001</v>
+        <v>-25.95</v>
       </c>
       <c r="M29" s="10">
-        <v>3.8499999999999091E-2</v>
+        <v>0.12700000000000067</v>
       </c>
       <c r="N29" s="14">
-        <v>48.1</v>
+        <v>59.89</v>
       </c>
       <c r="O29" s="1">
-        <v>2181.5538500000002</v>
+        <v>1820.3380999999999</v>
       </c>
       <c r="P29" s="1">
-        <v>0</v>
+        <v>8.66</v>
       </c>
       <c r="Q29" s="1">
-        <v>0</v>
+        <v>13</v>
       </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.25">
@@ -2039,111 +2032,156 @@
         <v>15</v>
       </c>
       <c r="C30" s="30">
-        <v>1380</v>
+        <v>1379</v>
       </c>
       <c r="D30" s="2">
-        <v>419</v>
+        <v>379.5</v>
       </c>
       <c r="E30" s="5">
-        <v>7.2999999999999995E-2</v>
+        <v>5.0999999999999997E-2</v>
       </c>
       <c r="F30" s="6">
-        <v>1.887</v>
+        <v>3.16</v>
       </c>
       <c r="G30" s="7">
         <f t="shared" si="2"/>
+        <v>14.905660377358492</v>
+      </c>
+      <c r="H30" s="5">
+        <v>0.21199999999999999</v>
+      </c>
+      <c r="I30" s="5">
+        <v>6.57</v>
+      </c>
+      <c r="J30" s="13">
+        <v>-26.973900000000008</v>
+      </c>
+      <c r="K30" s="13">
+        <v>1.4499999999999957E-2</v>
+      </c>
+      <c r="L30" s="10">
+        <v>-26.406500000000001</v>
+      </c>
+      <c r="M30" s="10">
+        <v>3.8499999999999091E-2</v>
+      </c>
+      <c r="N30" s="14">
+        <v>48.1</v>
+      </c>
+      <c r="O30" s="1">
+        <v>2181.5538500000002</v>
+      </c>
+      <c r="P30" s="1">
+        <v>8.84</v>
+      </c>
+      <c r="Q30" s="1">
+        <v>8.1999999999999993</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B31" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="C31" s="30">
+        <v>1380</v>
+      </c>
+      <c r="D31" s="2">
+        <v>419</v>
+      </c>
+      <c r="E31" s="5">
+        <v>7.2999999999999995E-2</v>
+      </c>
+      <c r="F31" s="6">
+        <v>1.887</v>
+      </c>
+      <c r="G31" s="7">
+        <f t="shared" si="2"/>
         <v>14.627906976744185</v>
       </c>
-      <c r="H30" s="5">
+      <c r="H31" s="5">
         <v>0.129</v>
       </c>
-      <c r="I30" s="5">
+      <c r="I31" s="5">
         <v>6.74</v>
       </c>
-      <c r="J30" s="13">
+      <c r="J31" s="13">
         <v>-26.642400000000002</v>
       </c>
-      <c r="K30" s="13">
+      <c r="K31" s="13">
         <v>4.699999999999882E-2</v>
       </c>
-      <c r="L30" s="10">
+      <c r="L31" s="10">
         <v>-26.226000000000003</v>
       </c>
-      <c r="M30" s="10">
+      <c r="M31" s="10">
         <v>7.949999999999946E-2</v>
       </c>
-      <c r="N30" s="14">
+      <c r="N31" s="14">
         <v>12.24</v>
       </c>
-      <c r="O30" s="1">
+      <c r="O31" s="1">
         <v>2455</v>
       </c>
-      <c r="P30" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q30" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:17" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="N32" s="21"/>
-    </row>
-    <row r="33" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D33" s="20"/>
-    </row>
-    <row r="34" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="P31" s="1">
+        <v>17.899999999999999</v>
+      </c>
+      <c r="Q31" s="1">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="33" spans="4:14" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="N33" s="21"/>
+    </row>
+    <row r="34" spans="4:14" x14ac:dyDescent="0.25">
       <c r="D34" s="20"/>
     </row>
-    <row r="35" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="4:14" x14ac:dyDescent="0.25">
       <c r="D35" s="20"/>
     </row>
-    <row r="36" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="4:14" x14ac:dyDescent="0.25">
       <c r="D36" s="20"/>
     </row>
-    <row r="37" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="4:14" x14ac:dyDescent="0.25">
       <c r="D37" s="20"/>
     </row>
-    <row r="38" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="4:14" x14ac:dyDescent="0.25">
       <c r="D38" s="20"/>
     </row>
-    <row r="39" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D39" s="2"/>
-    </row>
-    <row r="40" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D39" s="20"/>
+    </row>
+    <row r="40" spans="4:14" x14ac:dyDescent="0.25">
       <c r="D40" s="2"/>
     </row>
-    <row r="41" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="4:14" x14ac:dyDescent="0.25">
       <c r="D41" s="2"/>
     </row>
-    <row r="42" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="4:14" x14ac:dyDescent="0.25">
       <c r="D42" s="2"/>
     </row>
-    <row r="52" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D52" s="22"/>
-    </row>
-    <row r="67" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="F67" s="23"/>
-      <c r="G67" s="23"/>
-      <c r="H67" s="23"/>
-      <c r="I67" s="23"/>
+    <row r="43" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D43" s="2"/>
+    </row>
+    <row r="53" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D53" s="22"/>
     </row>
     <row r="68" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="E68" s="24"/>
-      <c r="F68" s="6"/>
-      <c r="G68" s="6"/>
-      <c r="H68" s="6"/>
-      <c r="I68" s="6"/>
-      <c r="K68" s="16"/>
-      <c r="L68" s="16"/>
+      <c r="F68" s="23"/>
+      <c r="G68" s="23"/>
+      <c r="H68" s="23"/>
+      <c r="I68" s="23"/>
     </row>
     <row r="69" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E69" s="24"/>
       <c r="F69" s="6"/>
       <c r="G69" s="6"/>
       <c r="H69" s="6"/>
       <c r="I69" s="6"/>
-      <c r="J69" s="10"/>
-      <c r="K69" s="10"/>
-      <c r="L69" s="10"/>
+      <c r="K69" s="16"/>
+      <c r="L69" s="16"/>
     </row>
     <row r="70" spans="5:12" x14ac:dyDescent="0.25">
       <c r="F70" s="6"/>
@@ -2230,7 +2268,7 @@
       <c r="F79" s="6"/>
       <c r="G79" s="6"/>
       <c r="H79" s="6"/>
-      <c r="I79" s="25"/>
+      <c r="I79" s="6"/>
       <c r="J79" s="10"/>
       <c r="K79" s="10"/>
       <c r="L79" s="10"/>
@@ -2239,32 +2277,32 @@
       <c r="F80" s="6"/>
       <c r="G80" s="6"/>
       <c r="H80" s="6"/>
-      <c r="I80" s="6"/>
+      <c r="I80" s="25"/>
       <c r="J80" s="10"/>
       <c r="K80" s="10"/>
       <c r="L80" s="10"/>
     </row>
     <row r="81" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="F81" s="10"/>
-      <c r="G81" s="10"/>
-      <c r="H81" s="10"/>
-      <c r="I81" s="10"/>
+      <c r="F81" s="6"/>
+      <c r="G81" s="6"/>
+      <c r="H81" s="6"/>
+      <c r="I81" s="6"/>
       <c r="J81" s="10"/>
       <c r="K81" s="10"/>
       <c r="L81" s="10"/>
     </row>
     <row r="82" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="F82" s="18"/>
-      <c r="G82" s="18"/>
-      <c r="H82" s="6"/>
-      <c r="I82" s="6"/>
+      <c r="F82" s="10"/>
+      <c r="G82" s="10"/>
+      <c r="H82" s="10"/>
+      <c r="I82" s="10"/>
       <c r="J82" s="10"/>
       <c r="K82" s="10"/>
       <c r="L82" s="10"/>
     </row>
     <row r="83" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="F83" s="6"/>
-      <c r="G83" s="6"/>
+      <c r="F83" s="18"/>
+      <c r="G83" s="18"/>
       <c r="H83" s="6"/>
       <c r="I83" s="6"/>
       <c r="J83" s="10"/>
@@ -2326,30 +2364,29 @@
       <c r="L89" s="10"/>
     </row>
     <row r="90" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="F90" s="6"/>
+      <c r="G90" s="6"/>
+      <c r="H90" s="6"/>
+      <c r="I90" s="6"/>
       <c r="J90" s="10"/>
+      <c r="K90" s="10"/>
+      <c r="L90" s="10"/>
     </row>
     <row r="91" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="F91" s="23"/>
-      <c r="G91" s="23"/>
-      <c r="H91" s="23"/>
-      <c r="I91" s="23"/>
+      <c r="J91" s="10"/>
     </row>
     <row r="92" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="E92" s="24"/>
-      <c r="F92" s="6"/>
-      <c r="G92" s="6"/>
-      <c r="H92" s="6"/>
-      <c r="I92" s="6"/>
+      <c r="F92" s="23"/>
+      <c r="G92" s="23"/>
+      <c r="H92" s="23"/>
+      <c r="I92" s="23"/>
     </row>
     <row r="93" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="E93" s="20"/>
+      <c r="E93" s="24"/>
       <c r="F93" s="6"/>
       <c r="G93" s="6"/>
       <c r="H93" s="6"/>
       <c r="I93" s="6"/>
-      <c r="J93" s="10"/>
-      <c r="K93" s="10"/>
-      <c r="L93" s="10"/>
     </row>
     <row r="94" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E94" s="20"/>
@@ -2402,7 +2439,7 @@
       <c r="L98" s="10"/>
     </row>
     <row r="99" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="E99" s="2"/>
+      <c r="E99" s="20"/>
       <c r="F99" s="6"/>
       <c r="G99" s="6"/>
       <c r="H99" s="6"/>
@@ -2433,9 +2470,19 @@
     </row>
     <row r="102" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E102" s="2"/>
+      <c r="F102" s="6"/>
+      <c r="G102" s="6"/>
+      <c r="H102" s="6"/>
+      <c r="I102" s="6"/>
       <c r="J102" s="10"/>
       <c r="K102" s="10"/>
       <c r="L102" s="10"/>
+    </row>
+    <row r="103" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E103" s="2"/>
+      <c r="J103" s="10"/>
+      <c r="K103" s="10"/>
+      <c r="L103" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>